<commit_message>
AdditionalCourseView inserts new data correspoding to users sheet
</commit_message>
<xml_diff>
--- a/res/StudentData.xlsx
+++ b/res/StudentData.xlsx
@@ -17,6 +17,7 @@
     <sheet name="loudiamond" r:id="rId2" sheetId="12"/>
     <sheet name="ian" r:id="rId3" sheetId="13"/>
     <sheet name="ruru" r:id="rId4" sheetId="14"/>
+    <sheet name="a" r:id="rId8" sheetId="15"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1510" uniqueCount="178">
   <si>
     <t>CS 111</t>
   </si>
@@ -526,6 +527,42 @@
   </si>
   <si>
     <t>Gen Math</t>
+  </si>
+  <si>
+    <t>Calc 1</t>
+  </si>
+  <si>
+    <t>Discrete Mathematics</t>
+  </si>
+  <si>
+    <t>90.0</t>
+  </si>
+  <si>
+    <t>AP Calc 1</t>
+  </si>
+  <si>
+    <t>Advance Placement Calculus</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>not yet taken</t>
+  </si>
+  <si>
+    <t>Alg 1</t>
+  </si>
+  <si>
+    <t>Linear Algebra</t>
   </si>
 </sst>
 </file>
@@ -1919,9 +1956,1582 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:G78"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B13" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B14" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B15" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B16" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B17" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B18" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B19" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B20" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B21" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B22" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B23" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B24" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B25" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B26" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B27" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B28" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B29" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B30" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" t="s">
+        <v>57</v>
+      </c>
+      <c r="E30" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B31" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C31" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B32" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B33" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E33" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F33" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B34" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C34" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B35" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C35" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" t="s">
+        <v>67</v>
+      </c>
+      <c r="E35" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F35" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B36" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F36" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B37" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>70</v>
+      </c>
+      <c r="D37" t="s">
+        <v>71</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F37" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B38" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C38" t="s">
+        <v>72</v>
+      </c>
+      <c r="D38" t="s">
+        <v>73</v>
+      </c>
+      <c r="E38" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F38" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B39" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C39" t="s">
+        <v>74</v>
+      </c>
+      <c r="D39" t="s">
+        <v>75</v>
+      </c>
+      <c r="E39" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F39" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B40" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>76</v>
+      </c>
+      <c r="D40" t="s">
+        <v>77</v>
+      </c>
+      <c r="E40" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F40" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B41" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C41" t="s">
+        <v>78</v>
+      </c>
+      <c r="D41" t="s">
+        <v>79</v>
+      </c>
+      <c r="E41" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F41" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B42" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C42" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" t="s">
+        <v>81</v>
+      </c>
+      <c r="E42" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F42" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B43" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C43" t="s">
+        <v>82</v>
+      </c>
+      <c r="D43" t="s">
+        <v>83</v>
+      </c>
+      <c r="E43" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F43" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B44" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C44" t="s">
+        <v>84</v>
+      </c>
+      <c r="D44" t="s">
+        <v>85</v>
+      </c>
+      <c r="E44" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F44" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B45" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C45" t="s">
+        <v>86</v>
+      </c>
+      <c r="D45" t="s">
+        <v>87</v>
+      </c>
+      <c r="E45" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F45" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B46" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C46" t="s">
+        <v>88</v>
+      </c>
+      <c r="D46" t="s">
+        <v>89</v>
+      </c>
+      <c r="E46" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F46" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B47" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C47" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47" t="s">
+        <v>91</v>
+      </c>
+      <c r="E47" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F47" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B48" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C48" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48" t="s">
+        <v>93</v>
+      </c>
+      <c r="E48" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F48" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B49" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C49" t="s">
+        <v>94</v>
+      </c>
+      <c r="D49" t="s">
+        <v>95</v>
+      </c>
+      <c r="E49" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F49" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B50" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C50" t="s">
+        <v>96</v>
+      </c>
+      <c r="D50" t="s">
+        <v>97</v>
+      </c>
+      <c r="E50" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F50" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B51" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C51" t="s">
+        <v>98</v>
+      </c>
+      <c r="D51" t="s">
+        <v>99</v>
+      </c>
+      <c r="E51" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F51" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B52" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C52" t="s">
+        <v>100</v>
+      </c>
+      <c r="D52" t="s">
+        <v>101</v>
+      </c>
+      <c r="E52" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F52" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B53" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C53" t="s">
+        <v>102</v>
+      </c>
+      <c r="D53" t="s">
+        <v>103</v>
+      </c>
+      <c r="E53" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F53" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B54" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C54" t="s">
+        <v>104</v>
+      </c>
+      <c r="D54" t="s">
+        <v>105</v>
+      </c>
+      <c r="E54" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F54" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B55" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C55" t="s">
+        <v>106</v>
+      </c>
+      <c r="D55" t="s">
+        <v>107</v>
+      </c>
+      <c r="E55" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F55" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B56" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C56" t="s">
+        <v>108</v>
+      </c>
+      <c r="D56" t="s">
+        <v>109</v>
+      </c>
+      <c r="E56" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F56" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B57" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>110</v>
+      </c>
+      <c r="D57" t="s">
+        <v>111</v>
+      </c>
+      <c r="E57" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F57" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B58" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C58" t="s">
+        <v>112</v>
+      </c>
+      <c r="D58" t="s">
+        <v>113</v>
+      </c>
+      <c r="E58" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F58" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B59" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C59" t="s">
+        <v>114</v>
+      </c>
+      <c r="D59" t="s">
+        <v>115</v>
+      </c>
+      <c r="E59" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F59" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B60" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C60" t="s">
+        <v>116</v>
+      </c>
+      <c r="D60" t="s">
+        <v>117</v>
+      </c>
+      <c r="E60" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F60" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B61" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C61" t="s">
+        <v>118</v>
+      </c>
+      <c r="D61" t="s">
+        <v>119</v>
+      </c>
+      <c r="E61" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F61" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B62" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C62" t="s">
+        <v>120</v>
+      </c>
+      <c r="D62" t="s">
+        <v>121</v>
+      </c>
+      <c r="E62" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F62" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B63" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C63" t="s">
+        <v>122</v>
+      </c>
+      <c r="D63" t="s">
+        <v>123</v>
+      </c>
+      <c r="E63" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F63" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B64" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C64" t="s">
+        <v>124</v>
+      </c>
+      <c r="D64" t="s">
+        <v>125</v>
+      </c>
+      <c r="E64" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F64" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B65" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C65" t="s">
+        <v>126</v>
+      </c>
+      <c r="D65" t="s">
+        <v>127</v>
+      </c>
+      <c r="E65" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="F65" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B66" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C66" t="s">
+        <v>128</v>
+      </c>
+      <c r="D66" t="s">
+        <v>129</v>
+      </c>
+      <c r="E66" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F66" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B67" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C67" t="s">
+        <v>130</v>
+      </c>
+      <c r="D67" t="s">
+        <v>131</v>
+      </c>
+      <c r="E67" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F67" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B68" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C68" t="s">
+        <v>132</v>
+      </c>
+      <c r="D68" t="s">
+        <v>133</v>
+      </c>
+      <c r="E68" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F68" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B69" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C69" t="s">
+        <v>134</v>
+      </c>
+      <c r="D69" t="s">
+        <v>135</v>
+      </c>
+      <c r="E69" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F69" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B70" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C70" t="s">
+        <v>136</v>
+      </c>
+      <c r="D70" t="s">
+        <v>137</v>
+      </c>
+      <c r="E70" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F70" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B71" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C71" t="s">
+        <v>136</v>
+      </c>
+      <c r="D71" t="s">
+        <v>138</v>
+      </c>
+      <c r="E71" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F71" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B72" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C72" t="s">
+        <v>139</v>
+      </c>
+      <c r="D72" t="s">
+        <v>129</v>
+      </c>
+      <c r="E72" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F72" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B73" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C73" t="s">
+        <v>140</v>
+      </c>
+      <c r="D73" t="s">
+        <v>141</v>
+      </c>
+      <c r="E73" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F73" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B74" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C74" t="s">
+        <v>142</v>
+      </c>
+      <c r="D74" t="s">
+        <v>143</v>
+      </c>
+      <c r="E74" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F74" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B75" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C75" t="s">
+        <v>144</v>
+      </c>
+      <c r="D75" t="s">
+        <v>145</v>
+      </c>
+      <c r="E75" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F75" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>171</v>
+      </c>
+      <c r="B76" t="s">
+        <v>171</v>
+      </c>
+      <c r="C76" t="s">
+        <v>173</v>
+      </c>
+      <c r="D76" t="s">
+        <v>174</v>
+      </c>
+      <c r="E76" t="s">
+        <v>155</v>
+      </c>
+      <c r="F76" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>171</v>
+      </c>
+      <c r="B77" t="s">
+        <v>171</v>
+      </c>
+      <c r="C77" t="s">
+        <v>169</v>
+      </c>
+      <c r="D77" t="s">
+        <v>170</v>
+      </c>
+      <c r="E77" t="s">
+        <v>155</v>
+      </c>
+      <c r="F77" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>171</v>
+      </c>
+      <c r="B78" t="s">
+        <v>171</v>
+      </c>
+      <c r="C78" t="s">
+        <v>176</v>
+      </c>
+      <c r="D78" t="s">
+        <v>177</v>
+      </c>
+      <c r="E78" t="s">
+        <v>155</v>
+      </c>
+      <c r="F78" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E65DC057-73A3-4661-A99B-97ABAA4E8D70}">
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
@@ -3429,6 +5039,16 @@
         <v>152</v>
       </c>
     </row>
+    <row r="76">
+      <c r="A76"/>
+      <c r="B76"/>
+      <c r="C76"/>
+      <c r="D76"/>
+      <c r="E76"/>
+      <c r="F76" t="s">
+        <v>171</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -3436,7 +5056,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3096677-D029-40D3-858D-169CD075D725}">
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
@@ -3472,7 +5092,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>166</v>
       </c>
       <c r="D2" t="s">
         <v>162</v>
@@ -3480,8 +5100,8 @@
       <c r="E2">
         <v>2</v>
       </c>
-      <c r="F2">
-        <v>90</v>
+      <c r="F2" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -3521,7 +5141,7 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -3555,7 +5175,7 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>167</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -4942,6 +6562,11 @@
       </c>
       <c r="F75" t="s">
         <v>152</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -4951,7 +6576,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7A51B6E-AB86-4AEA-B757-16C4749D4DB3}">
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6457,6 +8082,16 @@
         <v>152</v>
       </c>
     </row>
+    <row r="76">
+      <c r="A76"/>
+      <c r="B76"/>
+      <c r="C76"/>
+      <c r="D76"/>
+      <c r="E76"/>
+      <c r="F76" t="s">
+        <v>172</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Insert new data in the rows of table on SubjectWithGradesView
</commit_message>
<xml_diff>
--- a/res/StudentData.xlsx
+++ b/res/StudentData.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1510" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1540" uniqueCount="190">
   <si>
     <t>CS 111</t>
   </si>
@@ -563,6 +563,42 @@
   </si>
   <si>
     <t>Linear Algebra</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>79</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>test4</t>
+  </si>
+  <si>
+    <t>tesss</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>test5</t>
+  </si>
+  <si>
+    <t>tess</t>
+  </si>
+  <si>
+    <t>55</t>
   </si>
 </sst>
 </file>
@@ -1958,7 +1994,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G78"/>
+  <dimension ref="A1:G83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3522,6 +3558,106 @@
       </c>
       <c r="F78" t="s">
         <v>158</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>171</v>
+      </c>
+      <c r="B79" t="s">
+        <v>171</v>
+      </c>
+      <c r="C79" t="s">
+        <v>173</v>
+      </c>
+      <c r="D79" t="s">
+        <v>174</v>
+      </c>
+      <c r="E79" t="s">
+        <v>155</v>
+      </c>
+      <c r="F79" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>171</v>
+      </c>
+      <c r="B80" t="s">
+        <v>178</v>
+      </c>
+      <c r="C80" t="s">
+        <v>179</v>
+      </c>
+      <c r="D80" t="s">
+        <v>174</v>
+      </c>
+      <c r="E80" t="s">
+        <v>154</v>
+      </c>
+      <c r="F80" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>172</v>
+      </c>
+      <c r="B81" t="s">
+        <v>178</v>
+      </c>
+      <c r="C81" t="s">
+        <v>180</v>
+      </c>
+      <c r="D81" t="s">
+        <v>181</v>
+      </c>
+      <c r="E81" t="s">
+        <v>155</v>
+      </c>
+      <c r="F81" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>183</v>
+      </c>
+      <c r="B82" t="s">
+        <v>178</v>
+      </c>
+      <c r="C82" t="s">
+        <v>184</v>
+      </c>
+      <c r="D82" t="s">
+        <v>185</v>
+      </c>
+      <c r="E82" t="s">
+        <v>154</v>
+      </c>
+      <c r="F82" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>172</v>
+      </c>
+      <c r="B83" t="s">
+        <v>178</v>
+      </c>
+      <c r="C83" t="s">
+        <v>187</v>
+      </c>
+      <c r="D83" t="s">
+        <v>188</v>
+      </c>
+      <c r="E83" t="s">
+        <v>154</v>
+      </c>
+      <c r="F83" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a feature in which each View class communicates relating to user-data
</commit_message>
<xml_diff>
--- a/res/StudentData.xlsx
+++ b/res/StudentData.xlsx
@@ -18,6 +18,7 @@
     <sheet name="ian" r:id="rId3" sheetId="13"/>
     <sheet name="ruru" r:id="rId4" sheetId="14"/>
     <sheet name="a" r:id="rId8" sheetId="15"/>
+    <sheet name="b" r:id="rId9" sheetId="16"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1540" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2175" uniqueCount="230">
   <si>
     <t>CS 111</t>
   </si>
@@ -599,6 +600,126 @@
   </si>
   <si>
     <t>55</t>
+  </si>
+  <si>
+    <t>test11</t>
+  </si>
+  <si>
+    <t>test111</t>
+  </si>
+  <si>
+    <t>ttt</t>
+  </si>
+  <si>
+    <t>test22</t>
+  </si>
+  <si>
+    <t>test0</t>
+  </si>
+  <si>
+    <t>11.0</t>
+  </si>
+  <si>
+    <t>test00</t>
+  </si>
+  <si>
+    <t>testtest1</t>
+  </si>
+  <si>
+    <t>testest</t>
+  </si>
+  <si>
+    <t>testtest</t>
+  </si>
+  <si>
+    <t>jojbnjk</t>
+  </si>
+  <si>
+    <t>obiubiu</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>AA</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>test99</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>TEST1</t>
+  </si>
+  <si>
+    <t>NOT YET</t>
+  </si>
+  <si>
+    <t>53W</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>TESTING</t>
+  </si>
+  <si>
+    <t>NOT YET TAKEN</t>
+  </si>
+  <si>
+    <t>AAA</t>
+  </si>
+  <si>
+    <t>BBB</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>CCC</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>DDD</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>EEE</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>AP Calculus</t>
+  </si>
+  <si>
+    <t>AP Calculus 1</t>
+  </si>
+  <si>
+    <t>Calculus 1</t>
+  </si>
+  <si>
+    <t>Calculus 2</t>
+  </si>
+  <si>
+    <t>AP Calculus 2</t>
   </si>
 </sst>
 </file>
@@ -1994,7 +2115,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G83"/>
+  <dimension ref="A1:G99"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3658,6 +3779,1859 @@
       </c>
       <c r="F83" t="s">
         <v>189</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>178</v>
+      </c>
+      <c r="B84" t="s">
+        <v>178</v>
+      </c>
+      <c r="C84" t="s">
+        <v>190</v>
+      </c>
+      <c r="D84" t="s">
+        <v>174</v>
+      </c>
+      <c r="E84" t="s">
+        <v>155</v>
+      </c>
+      <c r="F84" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>172</v>
+      </c>
+      <c r="B85" t="s">
+        <v>178</v>
+      </c>
+      <c r="C85" t="s">
+        <v>191</v>
+      </c>
+      <c r="D85" t="s">
+        <v>181</v>
+      </c>
+      <c r="E85" t="s">
+        <v>155</v>
+      </c>
+      <c r="F85" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>178</v>
+      </c>
+      <c r="B86" t="s">
+        <v>178</v>
+      </c>
+      <c r="C86" t="s">
+        <v>193</v>
+      </c>
+      <c r="D86" t="s">
+        <v>193</v>
+      </c>
+      <c r="E86" t="s">
+        <v>155</v>
+      </c>
+      <c r="F86" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>172</v>
+      </c>
+      <c r="B87" t="s">
+        <v>178</v>
+      </c>
+      <c r="C87" t="s">
+        <v>194</v>
+      </c>
+      <c r="D87" t="s">
+        <v>181</v>
+      </c>
+      <c r="E87" t="s">
+        <v>195</v>
+      </c>
+      <c r="F87" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>172</v>
+      </c>
+      <c r="B88" t="s">
+        <v>178</v>
+      </c>
+      <c r="C88" t="s">
+        <v>196</v>
+      </c>
+      <c r="D88" t="s">
+        <v>181</v>
+      </c>
+      <c r="E88" t="s">
+        <v>155</v>
+      </c>
+      <c r="F88" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>172</v>
+      </c>
+      <c r="B89" t="s">
+        <v>178</v>
+      </c>
+      <c r="C89" t="s">
+        <v>197</v>
+      </c>
+      <c r="D89" t="s">
+        <v>198</v>
+      </c>
+      <c r="E89" t="s">
+        <v>155</v>
+      </c>
+      <c r="F89" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>178</v>
+      </c>
+      <c r="B90" t="s">
+        <v>178</v>
+      </c>
+      <c r="C90" t="s">
+        <v>201</v>
+      </c>
+      <c r="D90" t="s">
+        <v>200</v>
+      </c>
+      <c r="E90" t="s">
+        <v>155</v>
+      </c>
+      <c r="F90" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>172</v>
+      </c>
+      <c r="B91" t="s">
+        <v>178</v>
+      </c>
+      <c r="C91" t="s">
+        <v>173</v>
+      </c>
+      <c r="D91" t="s">
+        <v>199</v>
+      </c>
+      <c r="E91" t="s">
+        <v>155</v>
+      </c>
+      <c r="F91" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>178</v>
+      </c>
+      <c r="B92" t="s">
+        <v>178</v>
+      </c>
+      <c r="C92" t="s">
+        <v>202</v>
+      </c>
+      <c r="D92" t="s">
+        <v>204</v>
+      </c>
+      <c r="E92" t="s">
+        <v>155</v>
+      </c>
+      <c r="F92" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>171</v>
+      </c>
+      <c r="B93" t="s">
+        <v>178</v>
+      </c>
+      <c r="C93" t="s">
+        <v>205</v>
+      </c>
+      <c r="D93" t="s">
+        <v>205</v>
+      </c>
+      <c r="E93" t="s">
+        <v>153</v>
+      </c>
+      <c r="F93" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>172</v>
+      </c>
+      <c r="B94" t="s">
+        <v>178</v>
+      </c>
+      <c r="C94" t="s">
+        <v>206</v>
+      </c>
+      <c r="D94" t="s">
+        <v>206</v>
+      </c>
+      <c r="E94" t="s">
+        <v>153</v>
+      </c>
+      <c r="F94" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>172</v>
+      </c>
+      <c r="B95" t="s">
+        <v>178</v>
+      </c>
+      <c r="C95" t="s">
+        <v>207</v>
+      </c>
+      <c r="D95" t="s">
+        <v>208</v>
+      </c>
+      <c r="E95" t="s">
+        <v>155</v>
+      </c>
+      <c r="F95" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>178</v>
+      </c>
+      <c r="B96" t="s">
+        <v>178</v>
+      </c>
+      <c r="C96" t="s">
+        <v>173</v>
+      </c>
+      <c r="D96" t="s">
+        <v>181</v>
+      </c>
+      <c r="E96" t="s">
+        <v>155</v>
+      </c>
+      <c r="F96" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>171</v>
+      </c>
+      <c r="B97" t="s">
+        <v>171</v>
+      </c>
+      <c r="C97" t="s">
+        <v>208</v>
+      </c>
+      <c r="D97" t="s">
+        <v>209</v>
+      </c>
+      <c r="E97" t="s">
+        <v>155</v>
+      </c>
+      <c r="F97" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>172</v>
+      </c>
+      <c r="B98" t="s">
+        <v>178</v>
+      </c>
+      <c r="C98" t="s">
+        <v>208</v>
+      </c>
+      <c r="D98" t="s">
+        <v>213</v>
+      </c>
+      <c r="E98" t="s">
+        <v>155</v>
+      </c>
+      <c r="F98" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>172</v>
+      </c>
+      <c r="B99" t="s">
+        <v>178</v>
+      </c>
+      <c r="C99" t="s">
+        <v>222</v>
+      </c>
+      <c r="D99" t="s">
+        <v>223</v>
+      </c>
+      <c r="E99" t="s">
+        <v>155</v>
+      </c>
+      <c r="F99" t="s">
+        <v>186</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:G76"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B13" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B14" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B15" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B16" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B17" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B18" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B19" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B20" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B21" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B22" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B23" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B24" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B25" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B26" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B27" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B28" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B29" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B30" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" t="s">
+        <v>57</v>
+      </c>
+      <c r="E30" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B31" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C31" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B32" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B33" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E33" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F33" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B34" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C34" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B35" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C35" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" t="s">
+        <v>67</v>
+      </c>
+      <c r="E35" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F35" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B36" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F36" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B37" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>70</v>
+      </c>
+      <c r="D37" t="s">
+        <v>71</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F37" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B38" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C38" t="s">
+        <v>72</v>
+      </c>
+      <c r="D38" t="s">
+        <v>73</v>
+      </c>
+      <c r="E38" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F38" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B39" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C39" t="s">
+        <v>74</v>
+      </c>
+      <c r="D39" t="s">
+        <v>75</v>
+      </c>
+      <c r="E39" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F39" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B40" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>76</v>
+      </c>
+      <c r="D40" t="s">
+        <v>77</v>
+      </c>
+      <c r="E40" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F40" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B41" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C41" t="s">
+        <v>78</v>
+      </c>
+      <c r="D41" t="s">
+        <v>79</v>
+      </c>
+      <c r="E41" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F41" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B42" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C42" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" t="s">
+        <v>81</v>
+      </c>
+      <c r="E42" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F42" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B43" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C43" t="s">
+        <v>82</v>
+      </c>
+      <c r="D43" t="s">
+        <v>83</v>
+      </c>
+      <c r="E43" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F43" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B44" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C44" t="s">
+        <v>84</v>
+      </c>
+      <c r="D44" t="s">
+        <v>85</v>
+      </c>
+      <c r="E44" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F44" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B45" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C45" t="s">
+        <v>86</v>
+      </c>
+      <c r="D45" t="s">
+        <v>87</v>
+      </c>
+      <c r="E45" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F45" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B46" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C46" t="s">
+        <v>88</v>
+      </c>
+      <c r="D46" t="s">
+        <v>89</v>
+      </c>
+      <c r="E46" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F46" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B47" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C47" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47" t="s">
+        <v>91</v>
+      </c>
+      <c r="E47" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F47" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B48" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C48" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48" t="s">
+        <v>93</v>
+      </c>
+      <c r="E48" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F48" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B49" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C49" t="s">
+        <v>94</v>
+      </c>
+      <c r="D49" t="s">
+        <v>95</v>
+      </c>
+      <c r="E49" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F49" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B50" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C50" t="s">
+        <v>96</v>
+      </c>
+      <c r="D50" t="s">
+        <v>97</v>
+      </c>
+      <c r="E50" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F50" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B51" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C51" t="s">
+        <v>98</v>
+      </c>
+      <c r="D51" t="s">
+        <v>99</v>
+      </c>
+      <c r="E51" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F51" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B52" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C52" t="s">
+        <v>100</v>
+      </c>
+      <c r="D52" t="s">
+        <v>101</v>
+      </c>
+      <c r="E52" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F52" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B53" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C53" t="s">
+        <v>102</v>
+      </c>
+      <c r="D53" t="s">
+        <v>103</v>
+      </c>
+      <c r="E53" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F53" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B54" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C54" t="s">
+        <v>104</v>
+      </c>
+      <c r="D54" t="s">
+        <v>105</v>
+      </c>
+      <c r="E54" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F54" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B55" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C55" t="s">
+        <v>106</v>
+      </c>
+      <c r="D55" t="s">
+        <v>107</v>
+      </c>
+      <c r="E55" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F55" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B56" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C56" t="s">
+        <v>108</v>
+      </c>
+      <c r="D56" t="s">
+        <v>109</v>
+      </c>
+      <c r="E56" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F56" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B57" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>110</v>
+      </c>
+      <c r="D57" t="s">
+        <v>111</v>
+      </c>
+      <c r="E57" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F57" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B58" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C58" t="s">
+        <v>112</v>
+      </c>
+      <c r="D58" t="s">
+        <v>113</v>
+      </c>
+      <c r="E58" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F58" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B59" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C59" t="s">
+        <v>114</v>
+      </c>
+      <c r="D59" t="s">
+        <v>115</v>
+      </c>
+      <c r="E59" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F59" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B60" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C60" t="s">
+        <v>116</v>
+      </c>
+      <c r="D60" t="s">
+        <v>117</v>
+      </c>
+      <c r="E60" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F60" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B61" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C61" t="s">
+        <v>118</v>
+      </c>
+      <c r="D61" t="s">
+        <v>119</v>
+      </c>
+      <c r="E61" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F61" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B62" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C62" t="s">
+        <v>120</v>
+      </c>
+      <c r="D62" t="s">
+        <v>121</v>
+      </c>
+      <c r="E62" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F62" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B63" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C63" t="s">
+        <v>122</v>
+      </c>
+      <c r="D63" t="s">
+        <v>123</v>
+      </c>
+      <c r="E63" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F63" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B64" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C64" t="s">
+        <v>124</v>
+      </c>
+      <c r="D64" t="s">
+        <v>125</v>
+      </c>
+      <c r="E64" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F64" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B65" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C65" t="s">
+        <v>126</v>
+      </c>
+      <c r="D65" t="s">
+        <v>127</v>
+      </c>
+      <c r="E65" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="F65" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B66" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C66" t="s">
+        <v>128</v>
+      </c>
+      <c r="D66" t="s">
+        <v>129</v>
+      </c>
+      <c r="E66" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F66" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B67" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C67" t="s">
+        <v>130</v>
+      </c>
+      <c r="D67" t="s">
+        <v>131</v>
+      </c>
+      <c r="E67" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F67" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B68" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C68" t="s">
+        <v>132</v>
+      </c>
+      <c r="D68" t="s">
+        <v>133</v>
+      </c>
+      <c r="E68" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F68" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B69" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C69" t="s">
+        <v>134</v>
+      </c>
+      <c r="D69" t="s">
+        <v>135</v>
+      </c>
+      <c r="E69" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F69" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B70" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C70" t="s">
+        <v>136</v>
+      </c>
+      <c r="D70" t="s">
+        <v>137</v>
+      </c>
+      <c r="E70" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F70" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B71" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C71" t="s">
+        <v>136</v>
+      </c>
+      <c r="D71" t="s">
+        <v>138</v>
+      </c>
+      <c r="E71" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F71" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B72" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C72" t="s">
+        <v>139</v>
+      </c>
+      <c r="D72" t="s">
+        <v>129</v>
+      </c>
+      <c r="E72" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F72" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B73" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C73" t="s">
+        <v>140</v>
+      </c>
+      <c r="D73" t="s">
+        <v>141</v>
+      </c>
+      <c r="E73" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F73" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B74" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C74" t="s">
+        <v>142</v>
+      </c>
+      <c r="D74" t="s">
+        <v>143</v>
+      </c>
+      <c r="E74" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F74" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B75" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C75" t="s">
+        <v>144</v>
+      </c>
+      <c r="D75" t="s">
+        <v>145</v>
+      </c>
+      <c r="E75" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F75" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>171</v>
+      </c>
+      <c r="B76" t="s">
+        <v>171</v>
+      </c>
+      <c r="C76" t="s">
+        <v>229</v>
+      </c>
+      <c r="D76" t="s">
+        <v>228</v>
+      </c>
+      <c r="E76" t="s">
+        <v>155</v>
+      </c>
+      <c r="F76" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Security enchancement of user-login
</commit_message>
<xml_diff>
--- a/res/StudentData.xlsx
+++ b/res/StudentData.xlsx
@@ -19,6 +19,8 @@
     <sheet name="ruru" r:id="rId4" sheetId="14"/>
     <sheet name="a" r:id="rId8" sheetId="15"/>
     <sheet name="b" r:id="rId9" sheetId="16"/>
+    <sheet name="test0" r:id="rId10" sheetId="17"/>
+    <sheet name="loudz" r:id="rId11" sheetId="18"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2175" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3087" uniqueCount="230">
   <si>
     <t>CS 111</t>
   </si>
@@ -5639,6 +5641,3032 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:G75"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B13" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B14" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B15" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B16" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B17" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B18" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B19" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B20" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B21" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B22" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B23" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B24" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B25" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B26" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B27" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B28" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B29" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B30" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" t="s">
+        <v>57</v>
+      </c>
+      <c r="E30" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B31" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C31" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B32" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B33" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E33" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F33" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B34" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C34" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B35" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C35" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" t="s">
+        <v>67</v>
+      </c>
+      <c r="E35" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F35" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B36" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F36" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B37" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>70</v>
+      </c>
+      <c r="D37" t="s">
+        <v>71</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F37" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B38" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C38" t="s">
+        <v>72</v>
+      </c>
+      <c r="D38" t="s">
+        <v>73</v>
+      </c>
+      <c r="E38" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F38" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B39" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C39" t="s">
+        <v>74</v>
+      </c>
+      <c r="D39" t="s">
+        <v>75</v>
+      </c>
+      <c r="E39" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F39" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B40" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>76</v>
+      </c>
+      <c r="D40" t="s">
+        <v>77</v>
+      </c>
+      <c r="E40" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F40" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B41" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C41" t="s">
+        <v>78</v>
+      </c>
+      <c r="D41" t="s">
+        <v>79</v>
+      </c>
+      <c r="E41" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F41" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B42" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C42" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" t="s">
+        <v>81</v>
+      </c>
+      <c r="E42" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F42" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B43" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C43" t="s">
+        <v>82</v>
+      </c>
+      <c r="D43" t="s">
+        <v>83</v>
+      </c>
+      <c r="E43" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F43" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B44" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C44" t="s">
+        <v>84</v>
+      </c>
+      <c r="D44" t="s">
+        <v>85</v>
+      </c>
+      <c r="E44" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F44" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B45" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C45" t="s">
+        <v>86</v>
+      </c>
+      <c r="D45" t="s">
+        <v>87</v>
+      </c>
+      <c r="E45" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F45" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B46" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C46" t="s">
+        <v>88</v>
+      </c>
+      <c r="D46" t="s">
+        <v>89</v>
+      </c>
+      <c r="E46" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F46" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B47" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C47" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47" t="s">
+        <v>91</v>
+      </c>
+      <c r="E47" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F47" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B48" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C48" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48" t="s">
+        <v>93</v>
+      </c>
+      <c r="E48" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F48" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B49" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C49" t="s">
+        <v>94</v>
+      </c>
+      <c r="D49" t="s">
+        <v>95</v>
+      </c>
+      <c r="E49" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F49" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B50" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C50" t="s">
+        <v>96</v>
+      </c>
+      <c r="D50" t="s">
+        <v>97</v>
+      </c>
+      <c r="E50" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F50" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B51" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C51" t="s">
+        <v>98</v>
+      </c>
+      <c r="D51" t="s">
+        <v>99</v>
+      </c>
+      <c r="E51" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F51" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B52" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C52" t="s">
+        <v>100</v>
+      </c>
+      <c r="D52" t="s">
+        <v>101</v>
+      </c>
+      <c r="E52" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F52" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B53" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C53" t="s">
+        <v>102</v>
+      </c>
+      <c r="D53" t="s">
+        <v>103</v>
+      </c>
+      <c r="E53" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F53" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B54" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C54" t="s">
+        <v>104</v>
+      </c>
+      <c r="D54" t="s">
+        <v>105</v>
+      </c>
+      <c r="E54" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F54" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B55" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C55" t="s">
+        <v>106</v>
+      </c>
+      <c r="D55" t="s">
+        <v>107</v>
+      </c>
+      <c r="E55" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F55" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B56" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C56" t="s">
+        <v>108</v>
+      </c>
+      <c r="D56" t="s">
+        <v>109</v>
+      </c>
+      <c r="E56" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F56" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B57" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>110</v>
+      </c>
+      <c r="D57" t="s">
+        <v>111</v>
+      </c>
+      <c r="E57" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F57" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B58" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C58" t="s">
+        <v>112</v>
+      </c>
+      <c r="D58" t="s">
+        <v>113</v>
+      </c>
+      <c r="E58" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F58" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B59" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C59" t="s">
+        <v>114</v>
+      </c>
+      <c r="D59" t="s">
+        <v>115</v>
+      </c>
+      <c r="E59" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F59" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B60" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C60" t="s">
+        <v>116</v>
+      </c>
+      <c r="D60" t="s">
+        <v>117</v>
+      </c>
+      <c r="E60" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F60" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B61" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C61" t="s">
+        <v>118</v>
+      </c>
+      <c r="D61" t="s">
+        <v>119</v>
+      </c>
+      <c r="E61" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F61" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B62" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C62" t="s">
+        <v>120</v>
+      </c>
+      <c r="D62" t="s">
+        <v>121</v>
+      </c>
+      <c r="E62" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F62" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B63" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C63" t="s">
+        <v>122</v>
+      </c>
+      <c r="D63" t="s">
+        <v>123</v>
+      </c>
+      <c r="E63" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F63" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B64" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C64" t="s">
+        <v>124</v>
+      </c>
+      <c r="D64" t="s">
+        <v>125</v>
+      </c>
+      <c r="E64" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F64" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B65" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C65" t="s">
+        <v>126</v>
+      </c>
+      <c r="D65" t="s">
+        <v>127</v>
+      </c>
+      <c r="E65" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="F65" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B66" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C66" t="s">
+        <v>128</v>
+      </c>
+      <c r="D66" t="s">
+        <v>129</v>
+      </c>
+      <c r="E66" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F66" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B67" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C67" t="s">
+        <v>130</v>
+      </c>
+      <c r="D67" t="s">
+        <v>131</v>
+      </c>
+      <c r="E67" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F67" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B68" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C68" t="s">
+        <v>132</v>
+      </c>
+      <c r="D68" t="s">
+        <v>133</v>
+      </c>
+      <c r="E68" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F68" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B69" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C69" t="s">
+        <v>134</v>
+      </c>
+      <c r="D69" t="s">
+        <v>135</v>
+      </c>
+      <c r="E69" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F69" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B70" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C70" t="s">
+        <v>136</v>
+      </c>
+      <c r="D70" t="s">
+        <v>137</v>
+      </c>
+      <c r="E70" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F70" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B71" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C71" t="s">
+        <v>136</v>
+      </c>
+      <c r="D71" t="s">
+        <v>138</v>
+      </c>
+      <c r="E71" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F71" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B72" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C72" t="s">
+        <v>139</v>
+      </c>
+      <c r="D72" t="s">
+        <v>129</v>
+      </c>
+      <c r="E72" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F72" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B73" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C73" t="s">
+        <v>140</v>
+      </c>
+      <c r="D73" t="s">
+        <v>141</v>
+      </c>
+      <c r="E73" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F73" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B74" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C74" t="s">
+        <v>142</v>
+      </c>
+      <c r="D74" t="s">
+        <v>143</v>
+      </c>
+      <c r="E74" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F74" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B75" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C75" t="s">
+        <v>144</v>
+      </c>
+      <c r="D75" t="s">
+        <v>145</v>
+      </c>
+      <c r="E75" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F75" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:G75"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B13" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B14" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B15" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B16" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B17" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B18" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B19" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B20" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B21" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B22" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B23" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B24" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B25" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B26" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B27" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B28" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B29" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B30" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" t="s">
+        <v>57</v>
+      </c>
+      <c r="E30" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B31" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C31" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B32" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B33" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E33" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F33" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B34" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C34" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B35" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C35" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" t="s">
+        <v>67</v>
+      </c>
+      <c r="E35" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F35" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B36" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F36" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B37" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>70</v>
+      </c>
+      <c r="D37" t="s">
+        <v>71</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F37" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B38" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C38" t="s">
+        <v>72</v>
+      </c>
+      <c r="D38" t="s">
+        <v>73</v>
+      </c>
+      <c r="E38" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F38" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B39" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C39" t="s">
+        <v>74</v>
+      </c>
+      <c r="D39" t="s">
+        <v>75</v>
+      </c>
+      <c r="E39" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F39" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B40" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>76</v>
+      </c>
+      <c r="D40" t="s">
+        <v>77</v>
+      </c>
+      <c r="E40" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F40" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B41" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C41" t="s">
+        <v>78</v>
+      </c>
+      <c r="D41" t="s">
+        <v>79</v>
+      </c>
+      <c r="E41" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F41" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B42" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C42" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" t="s">
+        <v>81</v>
+      </c>
+      <c r="E42" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F42" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B43" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C43" t="s">
+        <v>82</v>
+      </c>
+      <c r="D43" t="s">
+        <v>83</v>
+      </c>
+      <c r="E43" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F43" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B44" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C44" t="s">
+        <v>84</v>
+      </c>
+      <c r="D44" t="s">
+        <v>85</v>
+      </c>
+      <c r="E44" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F44" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B45" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C45" t="s">
+        <v>86</v>
+      </c>
+      <c r="D45" t="s">
+        <v>87</v>
+      </c>
+      <c r="E45" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F45" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B46" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C46" t="s">
+        <v>88</v>
+      </c>
+      <c r="D46" t="s">
+        <v>89</v>
+      </c>
+      <c r="E46" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F46" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B47" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C47" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47" t="s">
+        <v>91</v>
+      </c>
+      <c r="E47" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F47" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B48" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C48" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48" t="s">
+        <v>93</v>
+      </c>
+      <c r="E48" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F48" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B49" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C49" t="s">
+        <v>94</v>
+      </c>
+      <c r="D49" t="s">
+        <v>95</v>
+      </c>
+      <c r="E49" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F49" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B50" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C50" t="s">
+        <v>96</v>
+      </c>
+      <c r="D50" t="s">
+        <v>97</v>
+      </c>
+      <c r="E50" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F50" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B51" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C51" t="s">
+        <v>98</v>
+      </c>
+      <c r="D51" t="s">
+        <v>99</v>
+      </c>
+      <c r="E51" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F51" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B52" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C52" t="s">
+        <v>100</v>
+      </c>
+      <c r="D52" t="s">
+        <v>101</v>
+      </c>
+      <c r="E52" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F52" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B53" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C53" t="s">
+        <v>102</v>
+      </c>
+      <c r="D53" t="s">
+        <v>103</v>
+      </c>
+      <c r="E53" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F53" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B54" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C54" t="s">
+        <v>104</v>
+      </c>
+      <c r="D54" t="s">
+        <v>105</v>
+      </c>
+      <c r="E54" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F54" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B55" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C55" t="s">
+        <v>106</v>
+      </c>
+      <c r="D55" t="s">
+        <v>107</v>
+      </c>
+      <c r="E55" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F55" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B56" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C56" t="s">
+        <v>108</v>
+      </c>
+      <c r="D56" t="s">
+        <v>109</v>
+      </c>
+      <c r="E56" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F56" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B57" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>110</v>
+      </c>
+      <c r="D57" t="s">
+        <v>111</v>
+      </c>
+      <c r="E57" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F57" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B58" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C58" t="s">
+        <v>112</v>
+      </c>
+      <c r="D58" t="s">
+        <v>113</v>
+      </c>
+      <c r="E58" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F58" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B59" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C59" t="s">
+        <v>114</v>
+      </c>
+      <c r="D59" t="s">
+        <v>115</v>
+      </c>
+      <c r="E59" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F59" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B60" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C60" t="s">
+        <v>116</v>
+      </c>
+      <c r="D60" t="s">
+        <v>117</v>
+      </c>
+      <c r="E60" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F60" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B61" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C61" t="s">
+        <v>118</v>
+      </c>
+      <c r="D61" t="s">
+        <v>119</v>
+      </c>
+      <c r="E61" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F61" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B62" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C62" t="s">
+        <v>120</v>
+      </c>
+      <c r="D62" t="s">
+        <v>121</v>
+      </c>
+      <c r="E62" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F62" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B63" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C63" t="s">
+        <v>122</v>
+      </c>
+      <c r="D63" t="s">
+        <v>123</v>
+      </c>
+      <c r="E63" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F63" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B64" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C64" t="s">
+        <v>124</v>
+      </c>
+      <c r="D64" t="s">
+        <v>125</v>
+      </c>
+      <c r="E64" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F64" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B65" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C65" t="s">
+        <v>126</v>
+      </c>
+      <c r="D65" t="s">
+        <v>127</v>
+      </c>
+      <c r="E65" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="F65" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B66" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C66" t="s">
+        <v>128</v>
+      </c>
+      <c r="D66" t="s">
+        <v>129</v>
+      </c>
+      <c r="E66" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F66" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B67" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C67" t="s">
+        <v>130</v>
+      </c>
+      <c r="D67" t="s">
+        <v>131</v>
+      </c>
+      <c r="E67" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F67" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B68" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C68" t="s">
+        <v>132</v>
+      </c>
+      <c r="D68" t="s">
+        <v>133</v>
+      </c>
+      <c r="E68" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F68" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B69" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C69" t="s">
+        <v>134</v>
+      </c>
+      <c r="D69" t="s">
+        <v>135</v>
+      </c>
+      <c r="E69" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F69" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B70" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C70" t="s">
+        <v>136</v>
+      </c>
+      <c r="D70" t="s">
+        <v>137</v>
+      </c>
+      <c r="E70" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F70" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B71" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C71" t="s">
+        <v>136</v>
+      </c>
+      <c r="D71" t="s">
+        <v>138</v>
+      </c>
+      <c r="E71" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F71" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B72" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C72" t="s">
+        <v>139</v>
+      </c>
+      <c r="D72" t="s">
+        <v>129</v>
+      </c>
+      <c r="E72" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F72" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B73" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C73" t="s">
+        <v>140</v>
+      </c>
+      <c r="D73" t="s">
+        <v>141</v>
+      </c>
+      <c r="E73" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F73" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B74" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C74" t="s">
+        <v>142</v>
+      </c>
+      <c r="D74" t="s">
+        <v>143</v>
+      </c>
+      <c r="E74" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F74" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B75" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C75" t="s">
+        <v>144</v>
+      </c>
+      <c r="D75" t="s">
+        <v>145</v>
+      </c>
+      <c r="E75" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F75" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E65DC057-73A3-4661-A99B-97ABAA4E8D70}">
   <dimension ref="A1:G76"/>

</xml_diff>

<commit_message>
Remodel the entire project, adding more complexity
</commit_message>
<xml_diff>
--- a/res/StudentData.xlsx
+++ b/res/StudentData.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loudi\IdeaProjects\_9315FinalGroupProject1\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C01279-55ED-4CCE-9223-B012680EBDF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{D7C01279-55ED-4CCE-9223-B012680EBDF2}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="12456" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
   </bookViews>
   <sheets>
-    <sheet name="test1" sheetId="11" r:id="rId1"/>
+    <sheet name="test1" r:id="rId1" sheetId="11"/>
+    <sheet name="test12" r:id="rId5" sheetId="12"/>
+    <sheet name="test123" r:id="rId6" sheetId="13"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="160">
   <si>
     <t>CS 111L</t>
   </si>
@@ -496,12 +498,22 @@
   </si>
   <si>
     <t>69</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>CS 111</t>
+  </si>
+  <si>
+    <t>Introduction to Computing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -529,16 +541,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -555,10 +567,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -593,7 +605,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -628,7 +640,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -722,21 +734,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -753,7 +765,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -805,15 +817,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2CB835A-8DA5-42B8-B44C-CF0933674699}">
-  <dimension ref="A1:F75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2CB835A-8DA5-42B8-B44C-CF0933674699}">
+  <dimension ref="A1:G75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
@@ -1884,6 +1896,3032 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:G75"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B13" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B14" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B15" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B16" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B17" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B18" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B19" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B20" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B21" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B22" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B23" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B24" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B25" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B26" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B27" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B28" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" t="s">
+        <v>51</v>
+      </c>
+      <c r="E28" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B29" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" t="s">
+        <v>53</v>
+      </c>
+      <c r="E29" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B30" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B31" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C31" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B32" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" t="s">
+        <v>59</v>
+      </c>
+      <c r="E32" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B33" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C33" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F33" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B34" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C34" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" t="s">
+        <v>63</v>
+      </c>
+      <c r="E34" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B35" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C35" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" t="s">
+        <v>65</v>
+      </c>
+      <c r="E35" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F35" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B36" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" t="s">
+        <v>67</v>
+      </c>
+      <c r="E36" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F36" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B37" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" t="s">
+        <v>69</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F37" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B38" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C38" t="s">
+        <v>70</v>
+      </c>
+      <c r="D38" t="s">
+        <v>71</v>
+      </c>
+      <c r="E38" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F38" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B39" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C39" t="s">
+        <v>72</v>
+      </c>
+      <c r="D39" t="s">
+        <v>73</v>
+      </c>
+      <c r="E39" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F39" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B40" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>74</v>
+      </c>
+      <c r="D40" t="s">
+        <v>75</v>
+      </c>
+      <c r="E40" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F40" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B41" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C41" t="s">
+        <v>76</v>
+      </c>
+      <c r="D41" t="s">
+        <v>77</v>
+      </c>
+      <c r="E41" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F41" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B42" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C42" t="s">
+        <v>78</v>
+      </c>
+      <c r="D42" t="s">
+        <v>79</v>
+      </c>
+      <c r="E42" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F42" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B43" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C43" t="s">
+        <v>80</v>
+      </c>
+      <c r="D43" t="s">
+        <v>81</v>
+      </c>
+      <c r="E43" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F43" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B44" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C44" t="s">
+        <v>82</v>
+      </c>
+      <c r="D44" t="s">
+        <v>83</v>
+      </c>
+      <c r="E44" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F44" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B45" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C45" t="s">
+        <v>84</v>
+      </c>
+      <c r="D45" t="s">
+        <v>85</v>
+      </c>
+      <c r="E45" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F45" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B46" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C46" t="s">
+        <v>86</v>
+      </c>
+      <c r="D46" t="s">
+        <v>87</v>
+      </c>
+      <c r="E46" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F46" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B47" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C47" t="s">
+        <v>88</v>
+      </c>
+      <c r="D47" t="s">
+        <v>89</v>
+      </c>
+      <c r="E47" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F47" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B48" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C48" t="s">
+        <v>90</v>
+      </c>
+      <c r="D48" t="s">
+        <v>91</v>
+      </c>
+      <c r="E48" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F48" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B49" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C49" t="s">
+        <v>92</v>
+      </c>
+      <c r="D49" t="s">
+        <v>93</v>
+      </c>
+      <c r="E49" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F49" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B50" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C50" t="s">
+        <v>94</v>
+      </c>
+      <c r="D50" t="s">
+        <v>95</v>
+      </c>
+      <c r="E50" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F50" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B51" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C51" t="s">
+        <v>96</v>
+      </c>
+      <c r="D51" t="s">
+        <v>97</v>
+      </c>
+      <c r="E51" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F51" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B52" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C52" t="s">
+        <v>98</v>
+      </c>
+      <c r="D52" t="s">
+        <v>99</v>
+      </c>
+      <c r="E52" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F52" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B53" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C53" t="s">
+        <v>100</v>
+      </c>
+      <c r="D53" t="s">
+        <v>101</v>
+      </c>
+      <c r="E53" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F53" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B54" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C54" t="s">
+        <v>102</v>
+      </c>
+      <c r="D54" t="s">
+        <v>103</v>
+      </c>
+      <c r="E54" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F54" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B55" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C55" t="s">
+        <v>104</v>
+      </c>
+      <c r="D55" t="s">
+        <v>105</v>
+      </c>
+      <c r="E55" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F55" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B56" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C56" t="s">
+        <v>106</v>
+      </c>
+      <c r="D56" t="s">
+        <v>107</v>
+      </c>
+      <c r="E56" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F56" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B57" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>108</v>
+      </c>
+      <c r="D57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E57" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F57" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B58" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C58" t="s">
+        <v>110</v>
+      </c>
+      <c r="D58" t="s">
+        <v>111</v>
+      </c>
+      <c r="E58" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F58" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B59" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C59" t="s">
+        <v>112</v>
+      </c>
+      <c r="D59" t="s">
+        <v>113</v>
+      </c>
+      <c r="E59" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F59" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B60" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C60" t="s">
+        <v>114</v>
+      </c>
+      <c r="D60" t="s">
+        <v>115</v>
+      </c>
+      <c r="E60" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F60" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B61" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C61" t="s">
+        <v>116</v>
+      </c>
+      <c r="D61" t="s">
+        <v>117</v>
+      </c>
+      <c r="E61" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F61" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B62" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C62" t="s">
+        <v>118</v>
+      </c>
+      <c r="D62" t="s">
+        <v>119</v>
+      </c>
+      <c r="E62" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F62" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B63" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C63" t="s">
+        <v>120</v>
+      </c>
+      <c r="D63" t="s">
+        <v>121</v>
+      </c>
+      <c r="E63" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F63" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B64" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C64" t="s">
+        <v>122</v>
+      </c>
+      <c r="D64" t="s">
+        <v>123</v>
+      </c>
+      <c r="E64" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F64" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B65" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C65" t="s">
+        <v>124</v>
+      </c>
+      <c r="D65" t="s">
+        <v>125</v>
+      </c>
+      <c r="E65" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="F65" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B66" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C66" t="s">
+        <v>126</v>
+      </c>
+      <c r="D66" t="s">
+        <v>127</v>
+      </c>
+      <c r="E66" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F66" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B67" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C67" t="s">
+        <v>128</v>
+      </c>
+      <c r="D67" t="s">
+        <v>129</v>
+      </c>
+      <c r="E67" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F67" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B68" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C68" t="s">
+        <v>130</v>
+      </c>
+      <c r="D68" t="s">
+        <v>131</v>
+      </c>
+      <c r="E68" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F68" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B69" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C69" t="s">
+        <v>132</v>
+      </c>
+      <c r="D69" t="s">
+        <v>133</v>
+      </c>
+      <c r="E69" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F69" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B70" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C70" t="s">
+        <v>134</v>
+      </c>
+      <c r="D70" t="s">
+        <v>135</v>
+      </c>
+      <c r="E70" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F70" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B71" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C71" t="s">
+        <v>134</v>
+      </c>
+      <c r="D71" t="s">
+        <v>136</v>
+      </c>
+      <c r="E71" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F71" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B72" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C72" t="s">
+        <v>137</v>
+      </c>
+      <c r="D72" t="s">
+        <v>127</v>
+      </c>
+      <c r="E72" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F72" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B73" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C73" t="s">
+        <v>138</v>
+      </c>
+      <c r="D73" t="s">
+        <v>139</v>
+      </c>
+      <c r="E73" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F73" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B74" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C74" t="s">
+        <v>140</v>
+      </c>
+      <c r="D74" t="s">
+        <v>141</v>
+      </c>
+      <c r="E74" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F74" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B75" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C75" t="s">
+        <v>142</v>
+      </c>
+      <c r="D75" t="s">
+        <v>143</v>
+      </c>
+      <c r="E75" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F75" t="s">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:G75"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B13" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B14" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B15" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B16" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B17" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B18" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B19" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B20" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B21" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B22" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B23" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B24" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B25" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B26" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B27" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B28" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" t="s">
+        <v>51</v>
+      </c>
+      <c r="E28" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B29" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" t="s">
+        <v>53</v>
+      </c>
+      <c r="E29" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B30" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B31" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C31" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B32" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" t="s">
+        <v>59</v>
+      </c>
+      <c r="E32" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B33" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C33" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F33" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B34" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C34" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" t="s">
+        <v>63</v>
+      </c>
+      <c r="E34" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B35" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C35" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" t="s">
+        <v>65</v>
+      </c>
+      <c r="E35" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F35" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B36" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" t="s">
+        <v>67</v>
+      </c>
+      <c r="E36" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F36" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B37" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" t="s">
+        <v>69</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F37" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B38" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C38" t="s">
+        <v>70</v>
+      </c>
+      <c r="D38" t="s">
+        <v>71</v>
+      </c>
+      <c r="E38" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F38" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B39" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C39" t="s">
+        <v>72</v>
+      </c>
+      <c r="D39" t="s">
+        <v>73</v>
+      </c>
+      <c r="E39" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F39" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B40" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>74</v>
+      </c>
+      <c r="D40" t="s">
+        <v>75</v>
+      </c>
+      <c r="E40" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F40" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B41" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C41" t="s">
+        <v>76</v>
+      </c>
+      <c r="D41" t="s">
+        <v>77</v>
+      </c>
+      <c r="E41" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F41" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B42" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C42" t="s">
+        <v>78</v>
+      </c>
+      <c r="D42" t="s">
+        <v>79</v>
+      </c>
+      <c r="E42" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F42" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B43" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C43" t="s">
+        <v>80</v>
+      </c>
+      <c r="D43" t="s">
+        <v>81</v>
+      </c>
+      <c r="E43" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F43" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B44" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C44" t="s">
+        <v>82</v>
+      </c>
+      <c r="D44" t="s">
+        <v>83</v>
+      </c>
+      <c r="E44" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F44" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B45" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C45" t="s">
+        <v>84</v>
+      </c>
+      <c r="D45" t="s">
+        <v>85</v>
+      </c>
+      <c r="E45" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F45" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B46" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C46" t="s">
+        <v>86</v>
+      </c>
+      <c r="D46" t="s">
+        <v>87</v>
+      </c>
+      <c r="E46" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F46" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B47" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C47" t="s">
+        <v>88</v>
+      </c>
+      <c r="D47" t="s">
+        <v>89</v>
+      </c>
+      <c r="E47" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F47" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B48" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C48" t="s">
+        <v>90</v>
+      </c>
+      <c r="D48" t="s">
+        <v>91</v>
+      </c>
+      <c r="E48" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F48" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B49" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C49" t="s">
+        <v>92</v>
+      </c>
+      <c r="D49" t="s">
+        <v>93</v>
+      </c>
+      <c r="E49" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F49" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B50" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C50" t="s">
+        <v>94</v>
+      </c>
+      <c r="D50" t="s">
+        <v>95</v>
+      </c>
+      <c r="E50" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F50" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B51" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C51" t="s">
+        <v>96</v>
+      </c>
+      <c r="D51" t="s">
+        <v>97</v>
+      </c>
+      <c r="E51" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F51" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B52" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C52" t="s">
+        <v>98</v>
+      </c>
+      <c r="D52" t="s">
+        <v>99</v>
+      </c>
+      <c r="E52" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F52" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B53" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C53" t="s">
+        <v>100</v>
+      </c>
+      <c r="D53" t="s">
+        <v>101</v>
+      </c>
+      <c r="E53" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F53" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B54" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C54" t="s">
+        <v>102</v>
+      </c>
+      <c r="D54" t="s">
+        <v>103</v>
+      </c>
+      <c r="E54" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F54" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B55" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C55" t="s">
+        <v>104</v>
+      </c>
+      <c r="D55" t="s">
+        <v>105</v>
+      </c>
+      <c r="E55" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F55" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B56" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C56" t="s">
+        <v>106</v>
+      </c>
+      <c r="D56" t="s">
+        <v>107</v>
+      </c>
+      <c r="E56" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F56" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B57" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>108</v>
+      </c>
+      <c r="D57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E57" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F57" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B58" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C58" t="s">
+        <v>110</v>
+      </c>
+      <c r="D58" t="s">
+        <v>111</v>
+      </c>
+      <c r="E58" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F58" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B59" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C59" t="s">
+        <v>112</v>
+      </c>
+      <c r="D59" t="s">
+        <v>113</v>
+      </c>
+      <c r="E59" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F59" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B60" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C60" t="s">
+        <v>114</v>
+      </c>
+      <c r="D60" t="s">
+        <v>115</v>
+      </c>
+      <c r="E60" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F60" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B61" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C61" t="s">
+        <v>116</v>
+      </c>
+      <c r="D61" t="s">
+        <v>117</v>
+      </c>
+      <c r="E61" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F61" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B62" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C62" t="s">
+        <v>118</v>
+      </c>
+      <c r="D62" t="s">
+        <v>119</v>
+      </c>
+      <c r="E62" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F62" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B63" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C63" t="s">
+        <v>120</v>
+      </c>
+      <c r="D63" t="s">
+        <v>121</v>
+      </c>
+      <c r="E63" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F63" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B64" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C64" t="s">
+        <v>122</v>
+      </c>
+      <c r="D64" t="s">
+        <v>123</v>
+      </c>
+      <c r="E64" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F64" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B65" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C65" t="s">
+        <v>124</v>
+      </c>
+      <c r="D65" t="s">
+        <v>125</v>
+      </c>
+      <c r="E65" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="F65" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B66" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C66" t="s">
+        <v>126</v>
+      </c>
+      <c r="D66" t="s">
+        <v>127</v>
+      </c>
+      <c r="E66" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F66" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B67" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C67" t="s">
+        <v>128</v>
+      </c>
+      <c r="D67" t="s">
+        <v>129</v>
+      </c>
+      <c r="E67" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F67" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B68" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C68" t="s">
+        <v>130</v>
+      </c>
+      <c r="D68" t="s">
+        <v>131</v>
+      </c>
+      <c r="E68" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F68" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B69" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C69" t="s">
+        <v>132</v>
+      </c>
+      <c r="D69" t="s">
+        <v>133</v>
+      </c>
+      <c r="E69" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F69" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B70" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C70" t="s">
+        <v>134</v>
+      </c>
+      <c r="D70" t="s">
+        <v>135</v>
+      </c>
+      <c r="E70" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F70" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B71" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C71" t="s">
+        <v>134</v>
+      </c>
+      <c r="D71" t="s">
+        <v>136</v>
+      </c>
+      <c r="E71" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F71" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B72" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C72" t="s">
+        <v>137</v>
+      </c>
+      <c r="D72" t="s">
+        <v>127</v>
+      </c>
+      <c r="E72" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F72" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B73" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C73" t="s">
+        <v>138</v>
+      </c>
+      <c r="D73" t="s">
+        <v>139</v>
+      </c>
+      <c r="E73" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F73" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B74" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C74" t="s">
+        <v>140</v>
+      </c>
+      <c r="D74" t="s">
+        <v>141</v>
+      </c>
+      <c r="E74" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F74" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B75" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C75" t="s">
+        <v>142</v>
+      </c>
+      <c r="D75" t="s">
+        <v>143</v>
+      </c>
+      <c r="E75" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F75" t="s">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>